<commit_message>
commit apr to apy
</commit_message>
<xml_diff>
--- a/calcul apr to apy.xlsx
+++ b/calcul apr to apy.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>APY = [1 + (APR / Number of Periods)]^(Number of Periods) - 1</t>
   </si>
@@ -92,13 +92,20 @@
   <si>
     <t>apr</t>
   </si>
+  <si>
+    <t>étape 1</t>
+  </si>
+  <si>
+    <t>étape 2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -171,7 +178,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -187,6 +194,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L31"/>
+  <dimension ref="A2:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -501,18 +509,18 @@
     <col min="11" max="11" width="14.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:14">
       <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="10"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:14">
       <c r="B8" t="s">
         <v>9</v>
       </c>
@@ -525,8 +533,23 @@
       <c r="E8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="I8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" t="s">
+        <v>15</v>
+      </c>
+      <c r="L8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="B9" s="2">
         <v>0.15</v>
       </c>
@@ -542,7 +565,7 @@
         <v>0.14999999999999991</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:14">
       <c r="B10" s="2">
         <v>0.15</v>
       </c>
@@ -558,7 +581,7 @@
         <v>0.1556249999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:14">
       <c r="B11" s="2">
         <v>0.15</v>
       </c>
@@ -573,7 +596,7 @@
         <v>0.16075451772299854</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:14">
       <c r="B12" s="2">
         <v>0.15</v>
       </c>
@@ -588,7 +611,7 @@
         <v>0.16158339378057973</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:14">
       <c r="B13" s="2">
         <v>0.15</v>
       </c>
@@ -602,6 +625,18 @@
         <f t="shared" si="0"/>
         <v>0.16179844312826397</v>
       </c>
+      <c r="I13">
+        <v>15</v>
+      </c>
+      <c r="J13">
+        <f>D13</f>
+        <v>365</v>
+      </c>
+      <c r="L13">
+        <f>1+(I13/100)</f>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="N13" s="11"/>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" s="9" t="s">

</xml_diff>